<commit_message>
Changes to avoid clobbering formulas on fast writes.
</commit_message>
<xml_diff>
--- a/NoSheetTests/TestData/SimpleWorkbook.xlsx
+++ b/NoSheetTests/TestData/SimpleWorkbook.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="24780" windowHeight="14700"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="20610" windowHeight="11640"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -352,7 +352,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -366,7 +366,7 @@
         <v>55</v>
       </c>
       <c r="C1">
-        <f>IF(B11&lt;B1,B11,B1)</f>
+        <f>IF(B1&lt;56,B11,B1)</f>
         <v>11</v>
       </c>
     </row>

</xml_diff>